<commit_message>
Changement des routes; suppression des fichiers inutiles au projet; Ajout du lien top sing-out; PowerPoint commencé.
</commit_message>
<xml_diff>
--- a/01_Conception/01_Dictionnaire_de_données/Dictionnaire_de_données.xlsx
+++ b/01_Conception/01_Dictionnaire_de_données/Dictionnaire_de_données.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomfouet/Library/Mobile Documents/com~apple~CloudDocs/LIDEM/11_TP/AIRBNB/01_Dictionnaire_de_données/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomfouet/Documents/Git/Github/TP/tp-Airbnb/01_Conception/01_Dictionnaire_de_données/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B404C4E-2607-B142-823E-36C647BA9E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62A5EC7-0B64-5F42-84B0-7CBAB17CF6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19440" xr2:uid="{8EB09076-4F5F-8247-A4A3-EF0FCC08E357}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" xr2:uid="{8EB09076-4F5F-8247-A4A3-EF0FCC08E357}"/>
   </bookViews>
   <sheets>
     <sheet name="MCD" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="81">
   <si>
     <t>Table</t>
   </si>
@@ -75,21 +75,9 @@
     <t>id_annonce</t>
   </si>
   <si>
-    <t>prix_annonce</t>
-  </si>
-  <si>
-    <t>taille_annonce</t>
-  </si>
-  <si>
-    <t>description_annonce</t>
-  </si>
-  <si>
     <t>equipements_annonce</t>
   </si>
   <si>
-    <t>couchages_annonce</t>
-  </si>
-  <si>
     <t>Identification unique du bien</t>
   </si>
   <si>
@@ -99,21 +87,12 @@
     <t>Identification unique de la réservation.</t>
   </si>
   <si>
-    <t>date_start_reservation</t>
-  </si>
-  <si>
-    <t>date_end_reservation</t>
-  </si>
-  <si>
     <t>Varchar</t>
   </si>
   <si>
     <t>Longueur</t>
   </si>
   <si>
-    <t>titre_annonce</t>
-  </si>
-  <si>
     <t>float</t>
   </si>
   <si>
@@ -132,12 +111,6 @@
     <t>id_annonceur</t>
   </si>
   <si>
-    <t>email_user</t>
-  </si>
-  <si>
-    <t>password_user</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -150,27 +123,12 @@
     <t>announcements</t>
   </si>
   <si>
-    <t>nom_user</t>
-  </si>
-  <si>
-    <t>tel_user</t>
-  </si>
-  <si>
-    <t>role_user</t>
-  </si>
-  <si>
     <t>Nombre de couchage du bien (max 150)</t>
   </si>
   <si>
-    <t>type_logements</t>
-  </si>
-  <si>
     <t>equipments</t>
   </si>
   <si>
-    <t>Boolean</t>
-  </si>
-  <si>
     <t>VARCHAR</t>
   </si>
   <si>
@@ -183,12 +141,6 @@
     <t>INTEGER</t>
   </si>
   <si>
-    <t>Pays où se trouve la location</t>
-  </si>
-  <si>
-    <t>Ville où se trouve la location</t>
-  </si>
-  <si>
     <t>Date de début de la réservation</t>
   </si>
   <si>
@@ -231,9 +183,6 @@
     <t>TABLES REFERENCES</t>
   </si>
   <si>
-    <t>prenom_user</t>
-  </si>
-  <si>
     <t>Mot de passe de l'utilisateur</t>
   </si>
   <si>
@@ -249,18 +198,12 @@
     <t>country</t>
   </si>
   <si>
-    <t>locations_logements</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
     <t>label</t>
   </si>
   <si>
-    <t>Commentaire</t>
-  </si>
-  <si>
     <t>Equipements (grille pain, …)</t>
   </si>
   <si>
@@ -268,6 +211,75 @@
   </si>
   <si>
     <t>id_logement</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>accommodations</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>surface</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>reservation</t>
+  </si>
+  <si>
+    <t>date_from</t>
+  </si>
+  <si>
+    <t>date_to</t>
+  </si>
+  <si>
+    <t>accommodation_types</t>
+  </si>
+  <si>
+    <t>addresses</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>Rue du bien</t>
+  </si>
+  <si>
+    <t>Ville où se trouve le bien</t>
+  </si>
+  <si>
+    <t>Pays où se trouve le bien</t>
+  </si>
+  <si>
+    <t>number_street</t>
+  </si>
+  <si>
+    <t>Numéro dans la rue où se trouve le bien</t>
   </si>
 </sst>
 </file>
@@ -426,8 +438,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8518925E-13D2-D14B-8161-734C3365AC4C}" name="Tableau1" displayName="Tableau1" ref="A2:F9" totalsRowShown="0">
-  <autoFilter ref="A2:F9" xr:uid="{8518925E-13D2-D14B-8161-734C3365AC4C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8518925E-13D2-D14B-8161-734C3365AC4C}" name="Tableau1" displayName="Tableau1" ref="A2:F10" totalsRowShown="0">
+  <autoFilter ref="A2:F10" xr:uid="{8518925E-13D2-D14B-8161-734C3365AC4C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CED540FC-94BB-B542-AB1F-BE14158F9F78}" name="Table"/>
     <tableColumn id="2" xr3:uid="{2303C49B-55AB-5942-92D5-A586A6F2E0A6}" name="Colonne"/>
@@ -456,8 +468,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2ECDC04-46F1-7245-988E-16F3D830E054}" name="Tableau4" displayName="Tableau4" ref="A21:F24" totalsRowShown="0">
-  <autoFilter ref="A21:F24" xr:uid="{C2ECDC04-46F1-7245-988E-16F3D830E054}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2ECDC04-46F1-7245-988E-16F3D830E054}" name="Tableau4" displayName="Tableau4" ref="A20:F23" totalsRowShown="0">
+  <autoFilter ref="A20:F23" xr:uid="{C2ECDC04-46F1-7245-988E-16F3D830E054}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E324162C-B0ED-9949-BB73-8FB4A91DD3DE}" name="Table"/>
     <tableColumn id="2" xr3:uid="{758E3243-167E-CB40-893C-D4005D6C03B4}" name="Colonne"/>
@@ -471,8 +483,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{32D9E716-8FA7-1D47-A5A6-27371DD64E6C}" name="Tableau2" displayName="Tableau2" ref="A28:F30" totalsRowShown="0">
-  <autoFilter ref="A28:F30" xr:uid="{32D9E716-8FA7-1D47-A5A6-27371DD64E6C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{32D9E716-8FA7-1D47-A5A6-27371DD64E6C}" name="Tableau2" displayName="Tableau2" ref="A26:F28" totalsRowShown="0">
+  <autoFilter ref="A26:F28" xr:uid="{32D9E716-8FA7-1D47-A5A6-27371DD64E6C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{6DA481E1-4887-2446-A7A4-360F5464F8E0}" name="Table"/>
     <tableColumn id="2" xr3:uid="{001824CF-E27A-9C44-8F02-EB181D137E4C}" name="Colonne"/>
@@ -486,8 +498,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CA43D181-9ACD-734F-8D8D-3D06238FC51B}" name="Tableau6" displayName="Tableau6" ref="A36:F38" totalsRowShown="0">
-  <autoFilter ref="A36:F38" xr:uid="{CA43D181-9ACD-734F-8D8D-3D06238FC51B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CA43D181-9ACD-734F-8D8D-3D06238FC51B}" name="Tableau6" displayName="Tableau6" ref="A30:F32" totalsRowShown="0">
+  <autoFilter ref="A30:F32" xr:uid="{CA43D181-9ACD-734F-8D8D-3D06238FC51B}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{F5D2E53B-020E-814A-8AF8-F9039F61EBF2}" name="Table"/>
     <tableColumn id="2" xr3:uid="{D45F1C75-00A7-5447-BBAA-ACE6ABD2F86F}" name="Colonne"/>
@@ -501,8 +513,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D3B1EC1A-18FC-CC42-97C5-1401F8BF3055}" name="Tableau7" displayName="Tableau7" ref="A43:F46" totalsRowShown="0">
-  <autoFilter ref="A43:F46" xr:uid="{D3B1EC1A-18FC-CC42-97C5-1401F8BF3055}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D3B1EC1A-18FC-CC42-97C5-1401F8BF3055}" name="Tableau7" displayName="Tableau7" ref="A34:F39" totalsRowShown="0">
+  <autoFilter ref="A34:F39" xr:uid="{D3B1EC1A-18FC-CC42-97C5-1401F8BF3055}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{FF38C67D-D7E1-2D40-A18F-7B9BCD49DBDF}" name="Table"/>
     <tableColumn id="2" xr3:uid="{2169CCBE-1A6F-B141-B5B3-0A7F0967F9C1}" name="Colonne"/>
@@ -862,16 +874,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE2E720E-C278-854D-89A6-000C03A656AA}">
-  <dimension ref="A1:H46"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.5" bestFit="1" customWidth="1"/>
@@ -880,7 +894,7 @@
     <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -891,7 +905,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -899,14 +913,8 @@
       <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -917,7 +925,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>3</v>
@@ -926,18 +934,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -946,88 +954,91 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D5">
+        <v>128</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
         <v>50</v>
       </c>
-      <c r="E5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>15</v>
-      </c>
       <c r="E6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D8">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1038,7 +1049,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>3</v>
@@ -1047,63 +1058,63 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D14">
         <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="3">
-        <v>255</v>
+        <v>18</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -1111,10 +1122,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="D17">
         <v>255</v>
@@ -1125,243 +1136,275 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>33</v>
+      </c>
+      <c r="D18">
+        <v>255</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>3</v>
+        <v>33</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>18</v>
-      </c>
       <c r="B22" t="s">
         <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
         <v>20</v>
       </c>
-      <c r="C23" t="s">
-        <v>27</v>
-      </c>
       <c r="E23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="E28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>0</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>1</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C30" t="s">
         <v>2</v>
       </c>
-      <c r="D28" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="6" t="s">
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="2" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30">
-        <v>100</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D31" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32">
+        <v>50</v>
+      </c>
+      <c r="E32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>74</v>
       </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>0</v>
-      </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F36" t="s">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="D36">
+        <v>50</v>
+      </c>
+      <c r="E36" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>41</v>
-      </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="D37">
+        <v>50</v>
+      </c>
+      <c r="E37" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="D38">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E38" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" t="s">
-        <v>23</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>69</v>
-      </c>
-      <c r="C45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D45">
-        <v>25</v>
-      </c>
-      <c r="E45" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>45</v>
-      </c>
-      <c r="C46" t="s">
-        <v>44</v>
-      </c>
-      <c r="D46">
-        <v>45</v>
-      </c>
-      <c r="E46" t="s">
-        <v>49</v>
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="82" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="6">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
@@ -1403,7 +1446,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -1412,7 +1455,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1426,7 +1469,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>3</v>
@@ -1437,58 +1480,58 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>50</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>50</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
         <v>22</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1502,7 +1545,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>3</v>
@@ -1513,16 +1556,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1530,14 +1573,15 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>

</xml_diff>